<commit_message>
Fix example data .xlsx
</commit_message>
<xml_diff>
--- a/mvts_analyzer/example/example_data.xlsx
+++ b/mvts_analyzer/example/example_data.xlsx
@@ -438,6 +438,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Index</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>DateTime</t>

</xml_diff>